<commit_message>
añadiendo archivo bluetooth y bluetooth2 para cada celular: monito y bebe respectivamente
</commit_message>
<xml_diff>
--- a/CuadoPatologia.xlsx
+++ b/CuadoPatologia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisi\Documents\Universidad\Tesis\Modelos_matematicos\sim_files_tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{928C2BE3-0255-48B5-80CC-B41758E17118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20258E1-C014-4107-8152-EE5B40F70AE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7AD7977E-B351-4C25-83AE-0DF9244F5BDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>presion</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>normal</t>
-  </si>
-  <si>
-    <t>60-100</t>
   </si>
   <si>
     <t>15-30</t>
@@ -528,7 +525,7 @@
   <dimension ref="A2:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,15 +540,15 @@
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
@@ -560,28 +557,28 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>1</v>
@@ -590,13 +587,13 @@
         <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>3</v>
@@ -610,51 +607,51 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>140</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
       <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
       <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" t="s">
         <v>9</v>
       </c>
-      <c r="K5" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>10</v>
-      </c>
-      <c r="O5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -663,23 +660,23 @@
         <v>0.3</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
         <v>34</v>
       </c>
-      <c r="M6" t="s">
-        <v>35</v>
-      </c>
       <c r="N6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
         <v>15</v>
-      </c>
-      <c r="O6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>